<commit_message>
2022 - Udgave 2
</commit_message>
<xml_diff>
--- a/en/BIMTypeCode - BDR - 2022DK.xlsx
+++ b/en/BIMTypeCode - BDR - 2022DK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cuboarkitekter.sharepoint.com/sites/BIM7AA/Shared Documents/BIMTypeCode/BIMTypeCode 2022 DK - Trin 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="900" documentId="13_ncr:1_{DAAC188B-F357-4D2F-88C6-4E03D0EEBA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E946BDB-EDF6-4CFB-9AD4-E5F050C09BA0}"/>
+  <xr:revisionPtr revIDLastSave="902" documentId="13_ncr:1_{DAAC188B-F357-4D2F-88C6-4E03D0EEBA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{160A7BB0-0C8E-46FC-AA06-2205B2B95E58}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2468" uniqueCount="749">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2469" uniqueCount="749">
   <si>
     <t xml:space="preserve">BIMTypeCode Detailing and Responsibility (BDR) schedule - by BIM7AA
 </t>
@@ -4015,6 +4015,55 @@
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4078,205 +4127,204 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="250">
-    <cellStyle name="Besøgt link" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Besøgt link" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Besøgt link" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Besøgt link" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Besøgt link" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="194" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="196" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="237" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="198" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="186" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="235" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="226" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="200" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="204" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="220" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="245" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="218" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="206" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="190" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="184" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="210" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="247" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="224" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="188" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="182" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="212" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="233" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="239" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="202" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="216" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="214" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="229" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="208" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="243" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="222" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="192" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="241" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="193" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="183" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="161" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="195" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="211" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="181" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="169" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="234" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="213" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="187" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="159" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="209" builtinId="8" hidden="1"/>
@@ -4284,7 +4332,6 @@
     <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="217" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="221" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
@@ -4292,7 +4339,6 @@
     <cellStyle name="Link" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="149" builtinId="8" hidden="1"/>
@@ -4300,81 +4346,35 @@
     <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="238" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="230" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="185" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="246" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="244" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="201" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="189" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="225" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="155" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="191" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="163" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="240" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="242" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="151" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="232" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="207" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="197" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="179" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="228" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="173" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="165" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="219" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="175" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="171" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="203" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="236" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="215" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="223" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="167" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="147" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="227" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
     <cellStyle name="Normal 3" xfId="248" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
@@ -7158,7 +7158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="X27:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
@@ -7190,8 +7190,8 @@
   </sheetPr>
   <dimension ref="A1:W396"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E402" sqref="E402"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -7209,19 +7209,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="29.25" customHeight="1">
-      <c r="B1" s="241" t="s">
+      <c r="B1" s="258" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="242"/>
-      <c r="D1" s="242"/>
-      <c r="E1" s="242"/>
-      <c r="F1" s="242"/>
-      <c r="G1" s="242"/>
-      <c r="H1" s="242"/>
-      <c r="I1" s="242"/>
-      <c r="J1" s="242"/>
-      <c r="K1" s="242"/>
-      <c r="L1" s="242"/>
+      <c r="C1" s="259"/>
+      <c r="D1" s="259"/>
+      <c r="E1" s="259"/>
+      <c r="F1" s="259"/>
+      <c r="G1" s="259"/>
+      <c r="H1" s="259"/>
+      <c r="I1" s="259"/>
+      <c r="J1" s="259"/>
+      <c r="K1" s="259"/>
+      <c r="L1" s="259"/>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="36.75" customHeight="1">
       <c r="A2" s="95"/>
@@ -7247,258 +7247,258 @@
         <v>6</v>
       </c>
       <c r="I2" s="208"/>
-      <c r="J2" s="243" t="s">
+      <c r="J2" s="260" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="244"/>
+      <c r="K2" s="261"/>
       <c r="L2" s="133" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1">
       <c r="A3" s="96"/>
-      <c r="B3" s="245" t="s">
+      <c r="B3" s="262" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="246"/>
+      <c r="C3" s="263"/>
       <c r="D3" s="101" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="212" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="250" t="s">
+      <c r="F3" s="267" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="251"/>
-      <c r="H3" s="256" t="s">
+      <c r="G3" s="268"/>
+      <c r="H3" s="273" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="257"/>
-      <c r="J3" s="257"/>
-      <c r="K3" s="258"/>
-      <c r="L3" s="259"/>
+      <c r="I3" s="274"/>
+      <c r="J3" s="274"/>
+      <c r="K3" s="275"/>
+      <c r="L3" s="276"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="96"/>
-      <c r="B4" s="245"/>
-      <c r="C4" s="247"/>
+      <c r="B4" s="262"/>
+      <c r="C4" s="264"/>
       <c r="D4" s="102" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="178" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="252"/>
-      <c r="G4" s="253"/>
+      <c r="F4" s="269"/>
+      <c r="G4" s="270"/>
       <c r="H4" s="97" t="s">
         <v>16</v>
       </c>
       <c r="I4" s="204"/>
-      <c r="J4" s="262" t="s">
+      <c r="J4" s="249" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="263"/>
-      <c r="L4" s="260"/>
+      <c r="K4" s="250"/>
+      <c r="L4" s="277"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1">
       <c r="A5" s="96"/>
-      <c r="B5" s="245"/>
-      <c r="C5" s="247"/>
+      <c r="B5" s="262"/>
+      <c r="C5" s="264"/>
       <c r="D5" s="102" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="179" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="252"/>
-      <c r="G5" s="253"/>
+      <c r="F5" s="269"/>
+      <c r="G5" s="270"/>
       <c r="H5" s="97" t="s">
         <v>20</v>
       </c>
       <c r="I5" s="204"/>
-      <c r="J5" s="262" t="s">
+      <c r="J5" s="249" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="263"/>
-      <c r="L5" s="260"/>
+      <c r="K5" s="250"/>
+      <c r="L5" s="277"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1">
       <c r="A6" s="96"/>
-      <c r="B6" s="245"/>
-      <c r="C6" s="247"/>
+      <c r="B6" s="262"/>
+      <c r="C6" s="264"/>
       <c r="D6" s="102" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="180" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="252"/>
-      <c r="G6" s="253"/>
+      <c r="F6" s="269"/>
+      <c r="G6" s="270"/>
       <c r="H6" s="97" t="s">
         <v>24</v>
       </c>
       <c r="I6" s="204"/>
-      <c r="J6" s="262" t="s">
+      <c r="J6" s="249" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="263"/>
-      <c r="L6" s="260"/>
+      <c r="K6" s="250"/>
+      <c r="L6" s="277"/>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1">
       <c r="A7" s="96"/>
-      <c r="B7" s="245"/>
-      <c r="C7" s="247"/>
+      <c r="B7" s="262"/>
+      <c r="C7" s="264"/>
       <c r="D7" s="102" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="181" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="252"/>
-      <c r="G7" s="253"/>
+      <c r="F7" s="269"/>
+      <c r="G7" s="270"/>
       <c r="H7" s="97" t="s">
         <v>28</v>
       </c>
       <c r="I7" s="204"/>
-      <c r="J7" s="262" t="s">
+      <c r="J7" s="249" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="263"/>
-      <c r="L7" s="260"/>
+      <c r="K7" s="250"/>
+      <c r="L7" s="277"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1">
       <c r="A8" s="96"/>
-      <c r="B8" s="245"/>
-      <c r="C8" s="247"/>
+      <c r="B8" s="262"/>
+      <c r="C8" s="264"/>
       <c r="D8" s="102" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="182" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="252"/>
-      <c r="G8" s="253"/>
+      <c r="F8" s="269"/>
+      <c r="G8" s="270"/>
       <c r="H8" s="97"/>
       <c r="I8" s="204"/>
-      <c r="J8" s="262"/>
-      <c r="K8" s="263"/>
-      <c r="L8" s="260"/>
+      <c r="J8" s="249"/>
+      <c r="K8" s="250"/>
+      <c r="L8" s="277"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1">
       <c r="A9" s="96"/>
-      <c r="B9" s="245"/>
-      <c r="C9" s="247"/>
+      <c r="B9" s="262"/>
+      <c r="C9" s="264"/>
       <c r="D9" s="102" t="s">
         <v>32</v>
       </c>
       <c r="E9" s="183" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="252"/>
-      <c r="G9" s="253"/>
+      <c r="F9" s="269"/>
+      <c r="G9" s="270"/>
       <c r="H9" s="98"/>
       <c r="I9" s="205"/>
-      <c r="J9" s="271"/>
-      <c r="K9" s="272"/>
-      <c r="L9" s="260"/>
+      <c r="J9" s="251"/>
+      <c r="K9" s="252"/>
+      <c r="L9" s="277"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="96"/>
-      <c r="B10" s="245"/>
-      <c r="C10" s="247"/>
+      <c r="B10" s="262"/>
+      <c r="C10" s="264"/>
       <c r="D10" s="102" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="184" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="252"/>
-      <c r="G10" s="253"/>
+      <c r="F10" s="269"/>
+      <c r="G10" s="270"/>
       <c r="H10" s="99"/>
       <c r="I10" s="206"/>
-      <c r="J10" s="273"/>
-      <c r="K10" s="274"/>
-      <c r="L10" s="260"/>
+      <c r="J10" s="253"/>
+      <c r="K10" s="254"/>
+      <c r="L10" s="277"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="96"/>
-      <c r="B11" s="245"/>
-      <c r="C11" s="247"/>
+      <c r="B11" s="262"/>
+      <c r="C11" s="264"/>
       <c r="D11" s="102" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="185" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="252"/>
-      <c r="G11" s="253"/>
+      <c r="F11" s="269"/>
+      <c r="G11" s="270"/>
       <c r="H11" s="98"/>
       <c r="I11" s="205"/>
-      <c r="J11" s="271"/>
-      <c r="K11" s="272"/>
-      <c r="L11" s="260"/>
+      <c r="J11" s="251"/>
+      <c r="K11" s="252"/>
+      <c r="L11" s="277"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="96"/>
-      <c r="B12" s="248"/>
-      <c r="C12" s="249"/>
+      <c r="B12" s="265"/>
+      <c r="C12" s="266"/>
       <c r="D12" s="103" t="s">
         <v>38</v>
       </c>
       <c r="E12" s="106" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="254"/>
-      <c r="G12" s="255"/>
+      <c r="F12" s="271"/>
+      <c r="G12" s="272"/>
       <c r="H12" s="100"/>
       <c r="I12" s="207"/>
-      <c r="J12" s="275"/>
-      <c r="K12" s="276"/>
-      <c r="L12" s="261"/>
+      <c r="J12" s="255"/>
+      <c r="K12" s="256"/>
+      <c r="L12" s="278"/>
     </row>
     <row r="13" spans="1:12" ht="10.5" customHeight="1" thickBot="1">
-      <c r="B13" s="277"/>
-      <c r="C13" s="277"/>
-      <c r="D13" s="277"/>
-      <c r="E13" s="277"/>
-      <c r="F13" s="277"/>
-      <c r="G13" s="277"/>
-      <c r="H13" s="277"/>
-      <c r="I13" s="277"/>
-      <c r="J13" s="277"/>
-      <c r="K13" s="277"/>
-      <c r="L13" s="277"/>
+      <c r="B13" s="257"/>
+      <c r="C13" s="257"/>
+      <c r="D13" s="257"/>
+      <c r="E13" s="257"/>
+      <c r="F13" s="257"/>
+      <c r="G13" s="257"/>
+      <c r="H13" s="257"/>
+      <c r="I13" s="257"/>
+      <c r="J13" s="257"/>
+      <c r="K13" s="257"/>
+      <c r="L13" s="257"/>
     </row>
     <row r="14" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B14" s="264" t="s">
+      <c r="B14" s="242" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="265"/>
-      <c r="D14" s="265"/>
-      <c r="E14" s="266"/>
-      <c r="F14" s="267" t="s">
+      <c r="C14" s="243"/>
+      <c r="D14" s="243"/>
+      <c r="E14" s="244"/>
+      <c r="F14" s="245" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="268"/>
-      <c r="H14" s="268"/>
-      <c r="I14" s="268"/>
-      <c r="J14" s="268"/>
-      <c r="K14" s="268"/>
-      <c r="L14" s="269"/>
+      <c r="G14" s="246"/>
+      <c r="H14" s="246"/>
+      <c r="I14" s="246"/>
+      <c r="J14" s="246"/>
+      <c r="K14" s="246"/>
+      <c r="L14" s="247"/>
     </row>
     <row r="15" spans="1:12" ht="9.75" customHeight="1" thickBot="1">
-      <c r="B15" s="270"/>
-      <c r="C15" s="270"/>
-      <c r="D15" s="270"/>
-      <c r="E15" s="270"/>
-      <c r="F15" s="270"/>
-      <c r="G15" s="270"/>
-      <c r="H15" s="270"/>
-      <c r="I15" s="270"/>
-      <c r="J15" s="270"/>
-      <c r="K15" s="270"/>
-      <c r="L15" s="270"/>
+      <c r="B15" s="248"/>
+      <c r="C15" s="248"/>
+      <c r="D15" s="248"/>
+      <c r="E15" s="248"/>
+      <c r="F15" s="248"/>
+      <c r="G15" s="248"/>
+      <c r="H15" s="248"/>
+      <c r="I15" s="248"/>
+      <c r="J15" s="248"/>
+      <c r="K15" s="248"/>
+      <c r="L15" s="248"/>
     </row>
     <row r="16" spans="1:12">
       <c r="B16" s="110" t="s">
@@ -7586,7 +7586,9 @@
       <c r="E19" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="117"/>
+      <c r="F19" s="13" t="s">
+        <v>16</v>
+      </c>
       <c r="G19" s="13" t="s">
         <v>20</v>
       </c>
@@ -17694,15 +17696,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:L14"/>
-    <mergeCell ref="B15:L15"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="B13:L13"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C12"/>
@@ -17713,6 +17706,15 @@
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:L14"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="B13:L13"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:E1 M1:XFD2 A2 A3:B3 D3:E7 M3:M12 O3:XFD12 A4:A12 E8 D9:E12 A13:E18 M13:XFD1048576 A19:A25 B24:B25 A26:E27 D28:E31 A28:C32 A33:E177 B178:E178 A178:A206 D179:E206 A207:E1048576">
     <cfRule type="cellIs" dxfId="45" priority="26" operator="equal">
@@ -17865,7 +17867,7 @@
       <c r="A2" s="237" t="s">
         <v>747</v>
       </c>
-      <c r="B2" s="278">
+      <c r="B2" s="241">
         <v>45089</v>
       </c>
       <c r="C2" s="237" t="s">
@@ -17874,22 +17876,22 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="237"/>
-      <c r="B3" s="278"/>
+      <c r="B3" s="241"/>
       <c r="C3" s="237"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="237"/>
-      <c r="B4" s="278"/>
+      <c r="B4" s="241"/>
       <c r="C4" s="237"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="237"/>
-      <c r="B5" s="278"/>
+      <c r="B5" s="241"/>
       <c r="C5" s="237"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="237"/>
-      <c r="B6" s="278"/>
+      <c r="B6" s="241"/>
       <c r="C6" s="159"/>
     </row>
     <row r="7" spans="1:3">
@@ -17902,6 +17904,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eb60fbdd-1e88-47bf-99c5-da0f6d3d8d0a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="45a28cd4-7f0b-475c-a950-133468d4a055" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100309FAFF55864F54C915D256FC93189CF" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fe1e7545a2d0d55fa1e8750be1390eca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="45a28cd4-7f0b-475c-a950-133468d4a055" xmlns:ns3="eb60fbdd-1e88-47bf-99c5-da0f6d3d8d0a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d2010749b15634dfb9f9de390013312" ns2:_="" ns3:_="">
     <xsd:import namespace="45a28cd4-7f0b-475c-a950-133468d4a055"/>
@@ -18132,17 +18145,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eb60fbdd-1e88-47bf-99c5-da0f6d3d8d0a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="45a28cd4-7f0b-475c-a950-133468d4a055" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -18153,11 +18155,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3050761F-C6E1-4173-BC0E-5C12741BAB73}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B699584-3BAF-4E02-9B52-D1E34ABD5E73}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B699584-3BAF-4E02-9B52-D1E34ABD5E73}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3050761F-C6E1-4173-BC0E-5C12741BAB73}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>